<commit_message>
updated BOM for parts used
</commit_message>
<xml_diff>
--- a/Documentation/BOM/TotalBOM_Final.xlsx
+++ b/Documentation/BOM/TotalBOM_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Received?</t>
+    <t xml:space="preserve">Used?</t>
   </si>
   <si>
     <t xml:space="preserve">Rechargeable 12 V Battery</t>
@@ -789,7 +789,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -810,7 +810,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -927,14 +927,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1268,11 +1260,11 @@
   </sheetPr>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="38.5"/>
@@ -1988,8 +1980,7 @@
         <f aca="false">Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
         <v>5.25</v>
       </c>
-      <c r="I23" s="5" t="b">
-        <f aca="false">TRUE()</f>
+      <c r="I23" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2019,8 +2010,7 @@
         <f aca="false">Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
         <v>25.9</v>
       </c>
-      <c r="I24" s="5" t="b">
-        <f aca="false">TRUE()</f>
+      <c r="I24" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2050,8 +2040,7 @@
         <f aca="false">Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
         <v>9.95</v>
       </c>
-      <c r="I25" s="5" t="b">
-        <f aca="false">TRUE()</f>
+      <c r="I25" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2081,8 +2070,7 @@
         <f aca="false">Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Price]]</f>
         <v>7.95</v>
       </c>
-      <c r="I26" s="5" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="I26" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3088,7 +3076,7 @@
   </sheetPr>
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -3099,7 +3087,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3375,33 +3363,33 @@
       <c r="E19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C20" s="36" t="n">
+      <c r="C20" s="23" t="n">
         <f aca="false">C4</f>
         <v>236.81</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="36" t="n">
+      <c r="E20" s="23" t="n">
         <f aca="false">C20</f>
         <v>236.81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="36" t="n">
+      <c r="C21" s="23" t="n">
         <f aca="false">C5</f>
         <v>185.96</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="36" t="n">
+      <c r="E21" s="23" t="n">
         <f aca="false">C21</f>
         <v>185.96</v>
       </c>

</xml_diff>